<commit_message>
psu status, health and power via xml implemented
</commit_message>
<xml_diff>
--- a/dell/passed/C1VV2S2_hwinvent_report_hw_passed_report.xlsx
+++ b/dell/passed/C1VV2S2_hwinvent_report_hw_passed_report.xlsx
@@ -13,8 +13,122 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author/>
+  </authors>
+  <commentList>
+    <comment ref="M2" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">"1" not equal golden setting "0" </t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="M3" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">"2" not equal golden setting "1" </t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="M4" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">"3" not equal golden setting "2" </t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="M5" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">"4" not equal golden setting "3" </t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="M6" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">"5" not equal golden setting "4" </t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="M7" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">"6" not equal golden setting "5" </t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="M8" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">"7" not equal golden setting "6" </t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="M9" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">"0" not equal golden setting "7" </t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="41">
   <si>
     <t>ServiceTag</t>
   </si>
@@ -31,7 +145,7 @@
     <t>Inventory date</t>
   </si>
   <si>
-    <t>20190102153433.000000+000</t>
+    <t>20190115214528.000000+000</t>
   </si>
   <si>
     <t>CPU model</t>
@@ -82,30 +196,30 @@
     <t>HDD serial</t>
   </si>
   <si>
+    <t>WFK1QAWD</t>
+  </si>
+  <si>
+    <t>WFK1Q9TT</t>
+  </si>
+  <si>
+    <t>WFK1QTH4</t>
+  </si>
+  <si>
+    <t>WFK1Q9Q7</t>
+  </si>
+  <si>
+    <t>WFK1Q9TY</t>
+  </si>
+  <si>
+    <t>WFK1QASM</t>
+  </si>
+  <si>
+    <t>WFK1QATA</t>
+  </si>
+  <si>
     <t>WFK1QAWX</t>
   </si>
   <si>
-    <t>WFK1QAWD</t>
-  </si>
-  <si>
-    <t>WFK1Q9TT</t>
-  </si>
-  <si>
-    <t>WFK1QTH4</t>
-  </si>
-  <si>
-    <t>WFK1Q9Q7</t>
-  </si>
-  <si>
-    <t>WFK1Q9TY</t>
-  </si>
-  <si>
-    <t>WFK1QASM</t>
-  </si>
-  <si>
-    <t>WFK1QATA</t>
-  </si>
-  <si>
     <t>HDD model</t>
   </si>
   <si>
@@ -115,6 +229,9 @@
     <t>HDD slot pop.</t>
   </si>
   <si>
+    <t>fail</t>
+  </si>
+  <si>
     <t>PSU P/Ns</t>
   </si>
   <si>
@@ -131,19 +248,28 @@
   </si>
   <si>
     <t>PSU fw</t>
+  </si>
+  <si>
+    <t>NIC status</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="4">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
@@ -163,6 +289,13 @@
     <font>
       <sz val="11"/>
       <color rgb="FF008000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -188,11 +321,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -487,7 +622,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:Q23"/>
+  <dimension ref="A1:R23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -510,382 +645,399 @@
     <col min="15" max="15" width="14.7109375" customWidth="1"/>
     <col min="16" max="16" width="9.7109375" customWidth="1"/>
     <col min="17" max="17" width="6.7109375" customWidth="1"/>
+    <col min="18" max="18" width="10.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:18">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="H1" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="I1" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="J1" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="K1" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="L1" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="M1" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="N1" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="O1" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="P1" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="Q1" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="R1" s="2" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="2" spans="1:18">
+      <c r="A2" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="H2" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="I2" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="J2" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="K2" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="L2" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="M2" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="O1" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="P1" s="1" t="s">
+      <c r="N2" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="O2" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="P2" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="Q2" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="R2" s="4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:18">
+      <c r="D3" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="H3" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="I3" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="J3" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="K3" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="L3" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="M3" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="N3" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="O3" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="Q1" s="1" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="2" spans="1:17">
-      <c r="A2" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="E2" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="F2" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="G2" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="H2" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="I2" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="J2" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="K2" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="L2" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="M2" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="N2" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="O2" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="P2" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="Q2" s="3" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="3" spans="1:17">
-      <c r="D3" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="E3" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="G3" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="H3" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="I3" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="J3" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="K3" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="L3" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="M3" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="N3" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="O3" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="P3" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="Q3" s="3" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="4" spans="1:17">
-      <c r="E4" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="G4" s="2" t="s">
+      <c r="P3" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="Q3" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="R3" s="4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:18">
+      <c r="E4" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="G4" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="H4" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="I4" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="J4" s="2" t="s">
+      <c r="H4" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="I4" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="J4" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="K4" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="L4" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="M4" s="3" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="5" spans="1:17">
-      <c r="E5" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="G5" s="2" t="s">
+      <c r="K4" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="L4" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="M4" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="R4" s="4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:18">
+      <c r="E5" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="G5" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="H5" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="I5" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="J5" s="2" t="s">
+      <c r="H5" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="I5" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="J5" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="K5" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="L5" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="M5" s="3" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="6" spans="1:17">
-      <c r="E6" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="G6" s="2" t="s">
+      <c r="K5" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="L5" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="M5" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="R5" s="4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6" spans="1:18">
+      <c r="E6" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="G6" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="H6" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="I6" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="J6" s="2" t="s">
+      <c r="H6" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="I6" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="J6" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="K6" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="L6" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="M6" s="3" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="7" spans="1:17">
-      <c r="E7" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="G7" s="2" t="s">
+      <c r="K6" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="L6" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="M6" s="5" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="7" spans="1:18">
+      <c r="E7" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="G7" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="H7" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="I7" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="J7" s="2" t="s">
+      <c r="H7" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="I7" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="J7" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="K7" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="L7" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="M7" s="3" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="8" spans="1:17">
-      <c r="E8" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="G8" s="2" t="s">
+      <c r="K7" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="L7" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="M7" s="5" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="8" spans="1:18">
+      <c r="E8" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="G8" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="H8" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="I8" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="J8" s="2" t="s">
+      <c r="H8" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="I8" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="J8" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="K8" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="L8" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="M8" s="3" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="9" spans="1:17">
-      <c r="E9" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="G9" s="2" t="s">
+      <c r="K8" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="L8" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="M8" s="5" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="9" spans="1:18">
+      <c r="E9" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="G9" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="H9" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="I9" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="J9" s="2" t="s">
+      <c r="H9" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="I9" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="J9" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="K9" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="L9" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="M9" s="3" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="10" spans="1:17">
-      <c r="E10" s="3" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="11" spans="1:17">
-      <c r="E11" s="3" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="12" spans="1:17">
-      <c r="E12" s="3" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="13" spans="1:17">
-      <c r="E13" s="3" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="14" spans="1:17">
-      <c r="E14" s="3" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="15" spans="1:17">
-      <c r="E15" s="3" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="16" spans="1:17">
-      <c r="E16" s="3" t="s">
+      <c r="K9" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="L9" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="M9" s="5" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="10" spans="1:18">
+      <c r="E10" s="4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="11" spans="1:18">
+      <c r="E11" s="4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="12" spans="1:18">
+      <c r="E12" s="4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="13" spans="1:18">
+      <c r="E13" s="4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="14" spans="1:18">
+      <c r="E14" s="4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="15" spans="1:18">
+      <c r="E15" s="4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="16" spans="1:18">
+      <c r="E16" s="4" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="17" spans="5:5">
-      <c r="E17" s="3" t="s">
+      <c r="E17" s="4" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="18" spans="5:5">
-      <c r="E18" s="3" t="s">
+      <c r="E18" s="4" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="19" spans="5:5">
-      <c r="E19" s="3" t="s">
+      <c r="E19" s="4" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="20" spans="5:5">
-      <c r="E20" s="3" t="s">
+      <c r="E20" s="4" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="21" spans="5:5">
-      <c r="E21" s="3" t="s">
+      <c r="E21" s="4" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="22" spans="5:5">
-      <c r="E22" s="3" t="s">
+      <c r="E22" s="4" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="23" spans="5:5">
-      <c r="E23" s="3" t="s">
+      <c r="E23" s="4" t="s">
         <v>7</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>